<commit_message>
Wrong Ids mapped in Corporation data
</commit_message>
<xml_diff>
--- a/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12354 Vasectomy/4. Vasectomy.xlsx
+++ b/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12354 Vasectomy/4. Vasectomy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="10350"/>
+    <workbookView windowWidth="23895" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -184,10 +184,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -244,6 +244,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -251,14 +266,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -267,22 +289,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,6 +311,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -304,69 +341,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,8 +372,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -408,187 +408,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,6 +679,71 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -702,71 +767,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -780,7 +780,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -798,130 +798,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1297,7 +1297,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>